<commit_message>
1. fixed typos 2. Give a detail information in concentration string values 3. updated function to support saliva samples 4. modified Alkane Standard related functions to support when it has not enough standard peaks
</commit_message>
<xml_diff>
--- a/lib/APGCMS/APGCMS/lib/lib_saliva_CalibrationCurve_20151112.xlsx
+++ b/lib/APGCMS/APGCMS/lib/lib_saliva_CalibrationCurve_20151112.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="134">
   <si>
     <t>SeqIndex</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Proline</t>
-  </si>
-  <si>
-    <t>Glycine-2</t>
   </si>
   <si>
     <t>HMDB00254</t>
@@ -1349,7 +1346,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1389,10 +1386,10 @@
       <c r="I1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1403,7 +1400,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="15">
         <v>3.73E-2</v>
@@ -1413,13 +1410,13 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M2" s="2">
         <v>14.366</v>
@@ -1443,13 +1440,13 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M3" s="2">
         <v>14.881</v>
@@ -1473,13 +1470,13 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M4" s="2">
         <v>16.172000000000001</v>
@@ -1507,7 +1504,7 @@
       <c r="I5" s="2"/>
       <c r="K5" s="6"/>
       <c r="L5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M5" s="2">
         <v>19.087</v>
@@ -1563,7 +1560,7 @@
       <c r="I7" s="2"/>
       <c r="K7" s="6"/>
       <c r="L7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M7" s="2">
         <v>20.388999999999999</v>
@@ -1591,7 +1588,7 @@
       <c r="I8" s="2"/>
       <c r="K8" s="6"/>
       <c r="L8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M8" s="2">
         <v>20.829000000000001</v>
@@ -1605,7 +1602,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="15">
         <v>8.8000000000000005E-3</v>
@@ -1619,7 +1616,7 @@
       <c r="I9" s="2"/>
       <c r="K9" s="6"/>
       <c r="L9" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M9" s="2">
         <v>21.013000000000002</v>
@@ -1630,10 +1627,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10" s="15">
         <v>-1.4500000000000001E-2</v>
@@ -1644,7 +1641,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I10" s="2">
         <v>20.829000000000001</v>
@@ -1675,13 +1672,13 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="K11" s="6"/>
       <c r="L11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M11" s="2">
         <v>21.289000000000001</v>
@@ -1709,7 +1706,7 @@
       <c r="I12" s="2"/>
       <c r="K12" s="6"/>
       <c r="L12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M12" s="2">
         <v>21.803000000000001</v>
@@ -1717,29 +1714,27 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" s="15">
-        <v>2.7199999999999998E-2</v>
+        <v>-1.7299999999999999E-2</v>
       </c>
       <c r="E13" s="15">
-        <v>1.6132</v>
+        <v>0.9</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M13" s="2">
         <v>22.122</v>
@@ -1747,27 +1742,29 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="15">
-        <v>-1.7299999999999999E-2</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0.9</v>
+      <c r="C14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="16">
+        <v>-9999</v>
+      </c>
+      <c r="E14" s="16">
+        <v>-9999</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="K14" s="6"/>
       <c r="L14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M14" s="2">
         <v>22.614000000000001</v>
@@ -1775,29 +1772,27 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="16">
-        <v>-9999</v>
-      </c>
-      <c r="E15" s="16">
-        <v>-9999</v>
+      <c r="C15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="15">
+        <v>-3.4799999999999998E-2</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.8</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="K15" s="6"/>
       <c r="L15" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M15" s="2">
         <v>23.015000000000001</v>
@@ -1805,19 +1800,19 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D16" s="15">
-        <v>-3.4799999999999998E-2</v>
+        <v>-2.24E-2</v>
       </c>
       <c r="E16" s="15">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1825,7 +1820,7 @@
       <c r="I16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M16" s="2">
         <v>23.550999999999998</v>
@@ -1833,19 +1828,19 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" s="15">
-        <v>-2.24E-2</v>
+        <v>-5.1999999999999998E-3</v>
       </c>
       <c r="E17" s="15">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1853,7 +1848,7 @@
       <c r="I17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M17" s="2">
         <v>24.097000000000001</v>
@@ -1861,27 +1856,29 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" s="15">
-        <v>-5.1999999999999998E-3</v>
+        <v>2.3099999999999999E-2</v>
       </c>
       <c r="E18" s="15">
-        <v>1.4</v>
+        <v>0.8891</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M18" s="2">
         <v>24.475999999999999</v>
@@ -1889,29 +1886,29 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="D19" s="15">
-        <v>2.3099999999999999E-2</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="E19" s="15">
-        <v>0.8891</v>
+        <v>1</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M19" s="2">
         <v>25.065000000000001</v>
@@ -1919,31 +1916,29 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>87</v>
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D20" s="15">
-        <v>-4.3999999999999997E-2</v>
+        <v>-3.8999999999999998E-3</v>
       </c>
       <c r="E20" s="15">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="K20" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M20" s="2">
         <v>25.19</v>
@@ -1951,19 +1946,19 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D21" s="15">
-        <v>-3.8999999999999998E-3</v>
+        <v>-2.9000000000000001E-2</v>
       </c>
       <c r="E21" s="15">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1971,7 +1966,7 @@
       <c r="I21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M21" s="2">
         <v>25.280999999999999</v>
@@ -1979,27 +1974,33 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>43</v>
+        <v>113</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="D22" s="15">
-        <v>-2.9000000000000001E-2</v>
+        <v>-5.3E-3</v>
       </c>
       <c r="E22" s="15">
-        <v>1.4</v>
+        <v>0.70630000000000004</v>
       </c>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="2">
+        <v>26.721</v>
+      </c>
       <c r="K22" s="2"/>
       <c r="L22" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M22" s="2">
         <v>25.829000000000001</v>
@@ -2007,33 +2008,27 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>94</v>
+        <v>43</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D23" s="15">
-        <v>-5.3E-3</v>
+        <v>-9.4999999999999998E-3</v>
       </c>
       <c r="E23" s="15">
-        <v>0.70630000000000004</v>
+        <v>1</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I23" s="2">
-        <v>26.721</v>
-      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M23" s="2">
         <v>26.721</v>
@@ -2041,29 +2036,31 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D24" s="15">
-        <v>-9.4999999999999998E-3</v>
+        <v>0.17380000000000001</v>
       </c>
       <c r="E24" s="15">
-        <v>1</v>
+        <v>1.7205999999999999</v>
       </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="K24" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M24" s="2">
         <v>26.992999999999999</v>
@@ -2071,29 +2068,29 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D25" s="15">
-        <v>0.17380000000000001</v>
+        <v>5.8299999999999998E-2</v>
       </c>
       <c r="E25" s="15">
-        <v>1.7205999999999999</v>
+        <v>3.7505099999999998</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M25" s="2">
         <v>27.216999999999999</v>
@@ -2101,29 +2098,27 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="15">
-        <v>5.8299999999999998E-2</v>
-      </c>
-      <c r="E26" s="15">
-        <v>3.7505099999999998</v>
+        <v>50</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2" t="s">
-        <v>120</v>
-      </c>
+      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M26" s="2">
         <v>28.233000000000001</v>
@@ -2131,19 +2126,19 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>52</v>
+        <v>71</v>
+      </c>
+      <c r="D27" s="15">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="E27" s="15">
+        <v>0.7</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -2151,7 +2146,7 @@
       <c r="I27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M27" s="2">
         <v>28.311</v>
@@ -2159,27 +2154,29 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D28" s="15">
-        <v>-3.6999999999999998E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
       <c r="E28" s="15">
-        <v>0.7</v>
+        <v>1.3006</v>
       </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M28" s="2">
         <v>28.716999999999999</v>
@@ -2187,31 +2184,29 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D29" s="15">
-        <v>8.4500000000000006E-2</v>
+        <v>-8.0399999999999999E-2</v>
       </c>
       <c r="E29" s="15">
-        <v>1.3006</v>
+        <v>2.5</v>
       </c>
       <c r="F29" s="2"/>
-      <c r="G29" s="2" t="s">
-        <v>120</v>
-      </c>
+      <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="K29" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M29" s="2">
         <v>29.658000000000001</v>
@@ -2219,27 +2214,31 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="D30" s="15">
-        <v>-8.0399999999999999E-2</v>
+        <v>-0.152</v>
       </c>
       <c r="E30" s="15">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="H30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I30" s="14">
+        <v>31.2</v>
+      </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M30" s="2">
         <v>29.747</v>
@@ -2247,34 +2246,30 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="D31" s="15">
-        <v>-0.152</v>
+        <v>-1.17E-2</v>
       </c>
       <c r="E31" s="15">
-        <v>3.6</v>
+        <v>1.8</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I31" s="14">
-        <v>31.2</v>
-      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
       <c r="J31" s="1"/>
       <c r="K31" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M31" s="2">
         <v>30.164000000000001</v>
@@ -2282,19 +2277,19 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D32" s="15">
-        <v>-1.17E-2</v>
+        <v>-3.1800000000000002E-2</v>
       </c>
       <c r="E32" s="15">
-        <v>1.8</v>
+        <v>3.5</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -2302,7 +2297,7 @@
       <c r="I32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M32" s="2">
         <v>31.2</v>
@@ -2310,29 +2305,31 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" s="15">
-        <v>-3.1800000000000002E-2</v>
+        <v>-7.5399999999999998E-3</v>
       </c>
       <c r="E33" s="15">
-        <v>3.5</v>
+        <v>0.68562999999999996</v>
       </c>
       <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="K33" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M33" s="2">
         <v>31.481000000000002</v>
@@ -2340,31 +2337,31 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D34" s="15">
-        <v>-7.5399999999999998E-3</v>
+        <v>1.4970000000000001E-2</v>
       </c>
       <c r="E34" s="15">
-        <v>0.68562999999999996</v>
+        <v>2.3371300000000002</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="K34" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M34" s="2">
         <v>32.170999999999999</v>
@@ -2372,29 +2369,33 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>63</v>
+        <v>35</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="D35" s="15">
-        <v>1.4970000000000001E-2</v>
+        <v>-7.5499999999999998E-2</v>
       </c>
       <c r="E35" s="15">
-        <v>2.3371300000000002</v>
+        <v>3.3555999999999999</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I35" s="2">
+        <v>33.159999999999997</v>
+      </c>
       <c r="K35" s="2"/>
       <c r="L35" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M35" s="2">
         <v>32.493000000000002</v>
@@ -2402,35 +2403,29 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="2">
-        <v>35</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>118</v>
+        <v>36</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D36" s="15">
-        <v>-7.5499999999999998E-2</v>
+        <v>-0.25209999999999999</v>
       </c>
       <c r="E36" s="15">
-        <v>3.3555999999999999</v>
+        <v>7.1</v>
       </c>
       <c r="F36" s="2"/>
-      <c r="G36" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="I36" s="2">
-        <v>33.159999999999997</v>
-      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
       <c r="K36" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M36" s="2">
         <v>32.908999999999999</v>
@@ -2438,29 +2433,31 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D37" s="15">
-        <v>-0.25209999999999999</v>
+        <v>-8.6199999999999999E-2</v>
       </c>
       <c r="E37" s="15">
-        <v>7.1</v>
+        <v>2.2332999999999998</v>
       </c>
       <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="K37" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M37" s="2">
         <v>33.159999999999997</v>
@@ -2468,29 +2465,27 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D38" s="15">
-        <v>-8.6199999999999999E-2</v>
+        <v>-0.22869999999999999</v>
       </c>
       <c r="E38" s="15">
-        <v>2.2332999999999998</v>
+        <v>4</v>
       </c>
       <c r="F38" s="2"/>
-      <c r="G38" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M38" s="2">
         <v>33.351999999999997</v>
@@ -2498,29 +2493,31 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D39" s="15">
-        <v>-0.22869999999999999</v>
+        <v>-6.7999999999999996E-3</v>
       </c>
       <c r="E39" s="15">
-        <v>4</v>
+        <v>0.59030000000000005</v>
       </c>
       <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="K39" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M39" s="2">
         <v>33.408000000000001</v>
@@ -2528,77 +2525,56 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D40" s="15">
-        <v>-6.7999999999999996E-3</v>
+        <v>-0.28260000000000002</v>
       </c>
       <c r="E40" s="15">
-        <v>0.59030000000000005</v>
+        <v>2.6</v>
       </c>
       <c r="F40" s="2"/>
-      <c r="G40" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="K40" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M40" s="2">
         <v>34.978000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="2">
-        <v>40</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="15">
-        <v>-0.28260000000000002</v>
-      </c>
-      <c r="E41" s="15">
-        <v>2.6</v>
-      </c>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M41" s="2">
         <v>35.052</v>
       </c>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M42" s="2">
         <v>35.295999999999999</v>
@@ -2607,7 +2583,7 @@
     <row r="43" spans="1:13">
       <c r="K43" s="2"/>
       <c r="L43" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M43" s="2">
         <v>35.427999999999997</v>
@@ -2615,10 +2591,10 @@
     </row>
     <row r="44" spans="1:13">
       <c r="K44" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M44" s="2">
         <v>38.710999999999999</v>
@@ -2626,10 +2602,10 @@
     </row>
     <row r="45" spans="1:13">
       <c r="K45" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M45" s="2">
         <v>38.856999999999999</v>

</xml_diff>